<commit_message>
Überarbeitung der Rechtschreibung in der Dokumentation Anpassung des Packetstruktur-Diagramms Architektur_Beschreibung noch in das Hauptverzeichnis der Anwendung kopiert
</commit_message>
<xml_diff>
--- a/JavaEE_Anforderungen.xlsx
+++ b/JavaEE_Anforderungen.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
   <si>
     <t>Komplexes Informationsobjekt (Listen, min 5 Attribute)</t>
   </si>
@@ -499,10 +499,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +804,7 @@
       </c>
       <c r="B1" s="25">
         <f>(SUM(C71:E71)*100)/SUM(C70:E70)</f>
-        <v>76.744186046511629</v>
+        <v>88.372093023255815</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>67</v>
@@ -816,7 +816,7 @@
       </c>
       <c r="B2" s="25">
         <f>C72</f>
-        <v>79.310344827586206</v>
+        <v>96.551724137931032</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>67</v>
@@ -1152,6 +1152,9 @@
       <c r="A33" t="s">
         <v>28</v>
       </c>
+      <c r="B33" s="25" t="s">
+        <v>64</v>
+      </c>
       <c r="C33" s="12" t="s">
         <v>64</v>
       </c>
@@ -1163,7 +1166,9 @@
       <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="28"/>
+      <c r="B34" s="29" t="s">
+        <v>64</v>
+      </c>
       <c r="C34" s="12" t="s">
         <v>64</v>
       </c>
@@ -1174,7 +1179,9 @@
       <c r="A35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="28"/>
+      <c r="B35" s="29" t="s">
+        <v>64</v>
+      </c>
       <c r="C35" s="12" t="s">
         <v>64</v>
       </c>
@@ -1185,7 +1192,9 @@
       <c r="A36" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="28"/>
+      <c r="B36" s="29" t="s">
+        <v>64</v>
+      </c>
       <c r="C36" s="12" t="s">
         <v>64</v>
       </c>
@@ -1196,7 +1205,9 @@
       <c r="A37" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="28"/>
+      <c r="B37" s="29" t="s">
+        <v>64</v>
+      </c>
       <c r="C37" s="12" t="s">
         <v>64</v>
       </c>
@@ -1207,7 +1218,9 @@
       <c r="A38" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="29"/>
+      <c r="B38" s="28" t="s">
+        <v>64</v>
+      </c>
       <c r="C38" s="12" t="s">
         <v>64</v>
       </c>
@@ -1509,9 +1522,6 @@
       <c r="A66" t="s">
         <v>58</v>
       </c>
-      <c r="B66" s="25" t="s">
-        <v>64</v>
-      </c>
       <c r="C66" s="12" t="s">
         <v>64</v>
       </c>
@@ -1557,7 +1567,7 @@
       </c>
       <c r="C71" s="8">
         <f>COUNTIFS($B$5:$B$69,"*",C5:C69,"x")</f>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D71" s="8">
         <f t="shared" ref="D71:E71" si="1">COUNTIFS($B$5:$B$69,"*",D5:D69,"x")</f>
@@ -1574,7 +1584,7 @@
       </c>
       <c r="C72" s="8">
         <f>(C71*100)/C70</f>
-        <v>79.310344827586206</v>
+        <v>96.551724137931032</v>
       </c>
       <c r="D72" s="8">
         <f t="shared" ref="D72:E72" si="2">(D71*100)/D70</f>

</xml_diff>